<commit_message>
Modificato captions2.xlsx <- è questo il file che utilizziamo per le descrizioni degli indicatori.
Il codice ora legge correttamente le varie captions.
</commit_message>
<xml_diff>
--- a/captions2.xlsx
+++ b/captions2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciglia88_ka/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/cstrozza_health_sdu_dk/Documents/_Other projects/StatisticAll 2021/IndicatoriDemografici/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE3ADFF-7E8A-B44E-8B7B-6ED9C92B145C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8DE3ADFF-7E8A-B44E-8B7B-6ED9C92B145C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD89FA4A-0CF4-424A-89E6-3672BCA2031C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28220" windowHeight="15080" xr2:uid="{8E01B10D-EA2E-4DD7-911D-41406BCBAA7F}"/>
+    <workbookView xWindow="8925" yWindow="2145" windowWidth="19395" windowHeight="11490" xr2:uid="{8E01B10D-EA2E-4DD7-911D-41406BCBAA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,78 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
-    <t xml:space="preserve">tasso di natalità (per mille abitanti)                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tasso di mortalità (per mille abitanti)                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tasso di nuzialità (per mille abitanti)                                 </t>
-  </si>
-  <si>
-    <t>speranza di vita a 65 anni - totale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saldo migratorio interno (per mille abitanti)                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">saldo migratorio con l'estero (per mille abitanti)                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">saldo migratorio per altro motivo (per mille abitanti)                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">saldo migratorio totale (per mille abitanti)                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">crescita naturale (per mille abitanti)                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tasso di crescita totale (per mille abitanti)                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">numero medio di figli per donna                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">età media della madre al parto                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita alla nascita - maschi                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita a 65 anni - maschi                                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita alla nascita - femmine                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita a 65 anni - femmine                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">popolazione 0-14 anni al 1° gennaio (valori percentuali) - al 1° gennaio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">popolazione 15-64 anni (valori percentuali) - al 1° gennaio              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">popolazione 65 anni e più (valori percentuali) - al 1° gennaio           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">indice di dipendenza strutturale (valori percentuali) - al 1° gennaio    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">indice di dipendenza degli anziani (valori percentuali) - al 1° gennaio  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">indice di vecchiaia (valori percentuali) - al 1° gennaio                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">età media della popolazione - al 1° gennaio                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita alla nascita - totale                                   </t>
-  </si>
-  <si>
     <t>Il tasso di mortalità indica il numero di persone morte in un anno ogni 1.000 abitanti. Esso viene calcolato con riferimento alla popolazione media dell'anno determinata sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo e dividendo il risultato per due.</t>
   </si>
   <si>
@@ -166,6 +94,78 @@
   </si>
   <si>
     <t>È l'età media della popolazione detenuta a una certa data, ottenuta dal rapporto tra la somma delle età di tutti gli individui e il numero degli individui, espressa in anni e decimi di anno.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasso di natalità (per mille abitanti)                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasso di mortalità (per mille abitanti)                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasso di nuzialità (per mille abitanti)                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo migratorio interno (per mille abitanti)                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo migratorio con l'estero (per mille abitanti)                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo migratorio per altro motivo (per mille abitanti)                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo migratorio totale (per mille abitanti)                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crescita naturale (per mille abitanti)                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasso di crescita totale (per mille abitanti)                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numero medio di figli per donna                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età media della madre al parto                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita alla nascita - maschi                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita a 65 anni - maschi                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita alla nascita - femmine                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita a 65 anni - femmine                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popolazione 0-14 anni al 1° gennaio (valori percentuali) - al 1° gennaio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popolazione 15-64 anni (valori percentuali) - al 1° gennaio              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popolazione 65 anni e più (valori percentuali) - al 1° gennaio           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indice di dipendenza strutturale (valori percentuali) - al 1° gennaio    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indice di dipendenza degli anziani (valori percentuali) - al 1° gennaio  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indice di vecchiaia (valori percentuali) - al 1° gennaio                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età media della popolazione - al 1° gennaio                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita alla nascita - totale                                   </t>
+  </si>
+  <si>
+    <t>Speranza di vita a 65 anni - totale</t>
   </si>
 </sst>
 </file>
@@ -209,13 +209,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -231,7 +230,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -529,208 +528,208 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC893BF-D5C5-4FA9-8452-D6FA45433575}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="134" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>